<commit_message>
Corrected white space in info sheet
</commit_message>
<xml_diff>
--- a/carbonPolicyShocks.xlsx
+++ b/carbonPolicyShocks.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dkaenzig\OneDrive - Northwestern University\Uni\LBS PhD\Research\Projects\Carbon tax\Repositories\CarbonShocks_laptop\Codes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nuwildcat-my.sharepoint.com/personal/drk9452_ads_northwestern_edu/Documents/Uni/LBS PhD/Research/Projects/Carbon tax/Repositories/carbonpolicyshocks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5EA9280-A2BF-46B7-A70A-AF7EEED6AEC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{F5EA9280-A2BF-46B7-A70A-AF7EEED6AEC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E4A1DC6C-B67F-4D44-8934-B34F9529F657}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="28800" windowHeight="15060" activeTab="1" xr2:uid="{C7087A5E-BA37-489A-AC63-C30DC6CCE652}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{C7087A5E-BA37-489A-AC63-C30DC6CCE652}"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline" sheetId="2" r:id="rId1"/>
@@ -3971,7 +3971,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3EE61EF-006E-43B0-BEA7-57EE2FFCBAA2}">
   <dimension ref="A1:C253"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:C253"/>
     </sheetView>
   </sheetViews>
@@ -6731,10 +6731,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFB91765-6434-41AE-B464-22B25C0FDAD7}">
-  <dimension ref="A19:C26"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6742,60 +6742,60 @@
     <col min="1" max="1" width="10.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B1" t="s">
         <v>256</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C1" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
         <v>258</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C2" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B4" t="s">
         <v>1</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C4" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
         <v>2</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C5" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B7" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B26" s="2" t="s">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B8" s="2" t="s">
         <v>265</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B26" r:id="rId1" xr:uid="{4BBAF1BB-DCDF-42B8-938D-AB6C075D458B}"/>
+    <hyperlink ref="B8" r:id="rId1" xr:uid="{4BBAF1BB-DCDF-42B8-938D-AB6C075D458B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>